<commit_message>
Updated API integration logic and added Pass/Fail functionality
</commit_message>
<xml_diff>
--- a/results_both_apis.xlsx
+++ b/results_both_apis.xlsx
@@ -640,7 +640,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/296937217728?mkevt=1&amp;mkcid=1&amp;mkrid=711-53200-19255-0&amp;campid=5337590632&amp;customid=&amp;toolid=10050&amp;amdata=enc%3AAQAJAAAAoHoV3kP08IDx%2BKZ9MfhVJKnEz9zHNm5Ys%2FHdWIwSYlOuE0BeX6GH42quGE3sSl5dAh3yLOztmq5Se9T3biG%2BqQB85eLZFQaduT5ORgF7lsKiMNQxRJGj%2BgFtqhd0qTuyrEgzftBcL5FCDAzNCQpFluUqz5f9ckMcPPqyzFCqU%2BK5QUvxUGM%2FhHT5Tg%2F%2BmqHYzhi%2FQJWnIJfgfxfopd%2BS7pM%3D</t>
+          <t>https://www.ebay.com/itm/296937217728?mkevt=1&amp;mkcid=1&amp;mkrid=711-53200-19255-0&amp;campid=5337590632&amp;customid=&amp;toolid=10050&amp;amdata=enc%3AAQAJAAAAoHoV3kP08IDx%2BKZ9MfhVJKnEz9zHNm5Ys%2FHdWIwSYlOuE0BeX6GH42quGE3sSl5dAlam%2FqZvibRWLVcjBwKi6IUOaFV5GX3l%2Bj04s5Aot6EAd%2BGaJiJr1c08bhUqXfdxCbYr5QRV3kSai%2BKpxHvLj9JelxSO5EdWyffuJcerVyzA0Hh9pxKEADS42qEi2F7JzOTMSn1hqO39yPnOlDpVZkc%3D</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/itm/296937217728?mkevt=1&amp;mkcid=1&amp;mkrid=711-53200-19255-0&amp;campid=5337590632&amp;customid=&amp;toolid=10050&amp;amdata=enc%3AAQAJAAAAoHoV3kP08IDx%2BKZ9MfhVJKnEz9zHNm5Ys%2FHdWIwSYlOuE0BeX6GH42quGE3sSl5dAlVfSKpEemZ2agfaM1FN%2BLUXO%2BReYhlG2ZfYxVTTKy%2FUZ3ZkZ%2Bii9li7FZaD8B3CzcgbqwKm0wB%2F3Is7tVPIR1nS3XZ0tt2%2Fjtzhd14SvRFhQnz56Kcmu3gk%2BGckiax8gIujPUaPweAXAgGQu7ZOWN8%3D</t>
+          <t>https://www.ebay.com/itm/296937217728?mkevt=1&amp;mkcid=1&amp;mkrid=711-53200-19255-0&amp;campid=5337590632&amp;customid=&amp;toolid=10050&amp;amdata=enc%3AAQAJAAAAoHoV3kP08IDx%2BKZ9MfhVJKnEz9zHNm5Ys%2FHdWIwSYlOuE0BeX6GH42quGE3sSl5dAiCxnXDmr9IV5hd3E1C2KBzXQ8BL2C3efD%2BEOYsq4nCfYTluATd%2BT%2BiBSqCSMQaMGv4bdpkqqyx7N5JDQB96OER4dlIseJjWB3Ftt6t66VlOkbccAwuz5cnapUpiwG6j6uLxgdqf7F8VJGhNZyhN2rw%3D</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>["https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40294/2__66737.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40293/Silver__85175.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40290/Black__60361.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40295/Green__35373.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40287/4__70292.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40288/3__05149.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40289/1__14954.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/224474/newmainpyp_54_62aa0b972b812987f4bda9f9__90767.1737979011.png?c=1"]</t>
+          <t>["https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40294/2__66737.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40293/Silver__85175.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40290/Black__60361.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40295/Green__35373.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40287/4__70292.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40288/3__05149.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40289/1__14954.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/224474/newmainpyp_54_62aa0b972b812987f4bda9f9__90767.1738031866.png?c=1"]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>["https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40294/2__66737.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40293/Silver__85175.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40290/Black__60361.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40295/Green__35373.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40287/4__70292.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40288/3__05149.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40289/1__14954.1737979011.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/224474/newmainpyp_54_62aa0b972b812987f4bda9f9__90767.1737979011.png?c=1"]</t>
+          <t>["https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40294/2__66737.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40293/Silver__85175.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40290/Black__60361.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40295/Green__35373.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40287/4__70292.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40288/3__05149.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/40289/1__14954.1738031866.jpg?c=1", "https://cdn11.bigcommerce.com/s-yqzpac968l/images/stencil/1280x1280/products/1954/224474/newmainpyp_54_62aa0b972b812987f4bda9f9__90767.1738031866.png?c=1"]</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>

</xml_diff>